<commit_message>
Tablas separadas por hoja en excel de informacion
</commit_message>
<xml_diff>
--- a/info-vinos_2023_v2.xlsx
+++ b/info-vinos_2023_v2.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eavanzin\Downloads\Elbio\universidad\Capstone\2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f50c2f2d00689fb9/Documentos/Universidad/2023-2/Capstone/Proyecto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A3FBF7-F742-4E87-8EAC-051D789BCC2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{63A3FBF7-F742-4E87-8EAC-051D789BCC2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A6C1C238-FE07-4970-A867-959065D5951E}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{9FE83E1C-AE4E-4FF0-90CF-2F394FA28AC8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{9FE83E1C-AE4E-4FF0-90CF-2F394FA28AC8}"/>
   </bookViews>
   <sheets>
     <sheet name="info 2023" sheetId="9" r:id="rId1"/>
     <sheet name="lotes " sheetId="8" r:id="rId2"/>
+    <sheet name="Hoja1" sheetId="10" r:id="rId3"/>
+    <sheet name="Hoja2" sheetId="11" r:id="rId4"/>
+    <sheet name="Hoja3" sheetId="12" r:id="rId5"/>
+    <sheet name="Hoja4" sheetId="13" r:id="rId6"/>
+    <sheet name="Hoja5" sheetId="14" r:id="rId7"/>
+    <sheet name="Hoja6" sheetId="15" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="348">
   <si>
     <t>Uva</t>
   </si>
@@ -1085,8 +1091,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -1143,10 +1149,10 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1157,16 +1163,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
@@ -1179,6 +1179,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1187,14 +1190,11 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Millares" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="2" builtinId="5"/>
+    <cellStyle name="Porcentaje" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1210,7 +1210,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1508,19 +1508,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{988F2DAE-07FB-46B3-A14C-238B483C364F}">
   <dimension ref="B2:M63"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="G60" sqref="G60"/>
+    <sheetView topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54:E63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="1"/>
     <col min="2" max="2" width="23.77734375" style="1" customWidth="1"/>
     <col min="3" max="3" width="13" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="17.109375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="12.77734375" style="4" customWidth="1"/>
-    <col min="7" max="7" width="12.88671875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="17.109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.77734375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="12.88671875" style="2" customWidth="1"/>
     <col min="8" max="8" width="11" style="1" customWidth="1"/>
     <col min="9" max="9" width="8.88671875" style="1"/>
     <col min="10" max="10" width="11.5546875" style="1" customWidth="1"/>
@@ -1539,16 +1539,15 @@
       <c r="C3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G3" s="4"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
@@ -1557,13 +1556,13 @@
       <c r="C4" s="1">
         <v>0.375</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="2">
         <v>0.5</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="2">
         <v>2</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="2">
         <v>2.875</v>
       </c>
     </row>
@@ -1574,13 +1573,13 @@
       <c r="C5" s="1">
         <v>0.375</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="2">
         <v>0.5</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="2">
         <v>1.5</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="2">
         <v>2.375</v>
       </c>
     </row>
@@ -1591,13 +1590,13 @@
       <c r="C6" s="1">
         <v>0.375</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="2">
         <v>0.35</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="2">
         <v>1.8250000000000002</v>
       </c>
     </row>
@@ -1608,13 +1607,13 @@
       <c r="C7" s="1">
         <v>0.375</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="2">
         <v>0.27</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="2">
         <v>0.9</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="2">
         <v>1.5449999999999999</v>
       </c>
     </row>
@@ -1625,16 +1624,16 @@
       <c r="C10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="2" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1645,16 +1644,16 @@
       <c r="C11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="2">
         <v>0.03</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="2">
         <v>0.02</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="2">
         <v>0.01</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="2">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
@@ -1665,16 +1664,16 @@
       <c r="C12" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="2">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="2">
         <v>1.2E-2</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="2">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="2">
         <v>2E-3</v>
       </c>
     </row>
@@ -1685,16 +1684,16 @@
       <c r="C13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="2">
         <v>0.03</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="2">
         <v>0.02</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="2">
         <v>0.01</v>
       </c>
-      <c r="G13" s="7">
+      <c r="G13" s="2">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
@@ -1705,16 +1704,16 @@
       <c r="C14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="2">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="2">
         <v>1.2E-2</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="2">
         <v>0.01</v>
       </c>
-      <c r="G14" s="7">
+      <c r="G14" s="2">
         <v>2E-3</v>
       </c>
     </row>
@@ -1725,16 +1724,16 @@
       <c r="C15" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="2">
         <v>0.03</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="2">
         <v>0.02</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="2">
         <v>0.01</v>
       </c>
-      <c r="G15" s="7">
+      <c r="G15" s="2">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
@@ -1745,16 +1744,16 @@
       <c r="C16" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="2">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="2">
         <v>1.2E-2</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="2">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="G16" s="7">
+      <c r="G16" s="2">
         <v>2E-3</v>
       </c>
     </row>
@@ -1765,13 +1764,13 @@
       <c r="C18" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F18" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1782,23 +1781,23 @@
       <c r="C19" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D19" s="4">
+      <c r="D19" s="2">
         <v>0.8</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E19" s="2">
         <v>0.85</v>
       </c>
-      <c r="F19" s="4">
+      <c r="F19" s="2">
         <v>0.95</v>
       </c>
-      <c r="H19" s="13" t="s">
+      <c r="H19" s="12" t="s">
         <v>346</v>
       </c>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
@@ -1807,21 +1806,21 @@
       <c r="C20" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D20" s="4">
+      <c r="D20" s="2">
         <v>0.75</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="2">
         <v>0.92</v>
       </c>
-      <c r="F20" s="4">
+      <c r="F20" s="2">
         <v>0.93</v>
       </c>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
@@ -1830,21 +1829,21 @@
       <c r="C21" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D21" s="2">
         <v>0.8</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E21" s="2">
         <v>0.91</v>
       </c>
-      <c r="F21" s="4">
+      <c r="F21" s="2">
         <v>0.87</v>
       </c>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="13"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
@@ -1853,21 +1852,21 @@
       <c r="C22" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D22" s="2">
         <v>0.7</v>
       </c>
-      <c r="E22" s="4">
+      <c r="E22" s="2">
         <v>0.95</v>
       </c>
-      <c r="F22" s="4">
+      <c r="F22" s="2">
         <v>0.95</v>
       </c>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
@@ -1876,21 +1875,21 @@
       <c r="C23" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D23" s="2">
         <v>0.8</v>
       </c>
-      <c r="E23" s="4">
+      <c r="E23" s="2">
         <v>0.85</v>
       </c>
-      <c r="F23" s="4">
+      <c r="F23" s="2">
         <v>0.85</v>
       </c>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
@@ -1899,25 +1898,25 @@
       <c r="C24" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="4">
+      <c r="D24" s="2">
         <v>0.7</v>
       </c>
-      <c r="E24" s="4">
+      <c r="E24" s="2">
         <v>0.93</v>
       </c>
-      <c r="F24" s="4">
+      <c r="F24" s="2">
         <v>0.94</v>
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="D26" s="11" t="s">
+      <c r="D26" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
@@ -1926,16 +1925,16 @@
       <c r="C27" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E27" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F27" s="4" t="s">
+      <c r="F27" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G27" s="4" t="s">
+      <c r="G27" s="2" t="s">
         <v>24</v>
       </c>
       <c r="H27" s="1" t="s">
@@ -1952,13 +1951,13 @@
       <c r="C28" s="1">
         <v>1</v>
       </c>
-      <c r="D28" s="4">
+      <c r="D28" s="2">
         <v>0.1</v>
       </c>
-      <c r="E28" s="4">
+      <c r="E28" s="2">
         <v>0.2</v>
       </c>
-      <c r="G28" s="4">
+      <c r="G28" s="2">
         <v>0.3</v>
       </c>
       <c r="I28" s="1">
@@ -1969,13 +1968,13 @@
       <c r="C29" s="1">
         <v>2</v>
       </c>
-      <c r="E29" s="4">
+      <c r="E29" s="2">
         <v>0.4</v>
       </c>
-      <c r="F29" s="4">
+      <c r="F29" s="2">
         <v>0.2</v>
       </c>
-      <c r="G29" s="4">
+      <c r="G29" s="2">
         <v>0.2</v>
       </c>
       <c r="I29" s="1">
@@ -1989,16 +1988,16 @@
       <c r="C30" s="1">
         <v>1</v>
       </c>
-      <c r="D30" s="4">
+      <c r="D30" s="2">
         <v>0.3</v>
       </c>
-      <c r="E30" s="4">
+      <c r="E30" s="2">
         <v>0.2</v>
       </c>
-      <c r="F30" s="4">
+      <c r="F30" s="2">
         <v>0.1</v>
       </c>
-      <c r="G30" s="4">
+      <c r="G30" s="2">
         <v>0.2</v>
       </c>
       <c r="I30" s="1">
@@ -2009,13 +2008,13 @@
       <c r="C31" s="1">
         <v>2</v>
       </c>
-      <c r="E31" s="4">
+      <c r="E31" s="2">
         <v>0.2</v>
       </c>
-      <c r="F31" s="4">
+      <c r="F31" s="2">
         <v>0.2</v>
       </c>
-      <c r="G31" s="4">
+      <c r="G31" s="2">
         <v>0.2</v>
       </c>
       <c r="H31" s="1">
@@ -2029,13 +2028,13 @@
       <c r="C32" s="1">
         <v>3</v>
       </c>
-      <c r="D32" s="4">
+      <c r="D32" s="2">
         <v>0.2</v>
       </c>
-      <c r="F32" s="4">
+      <c r="F32" s="2">
         <v>0.2</v>
       </c>
-      <c r="G32" s="4">
+      <c r="G32" s="2">
         <v>0.2</v>
       </c>
       <c r="I32" s="1">
@@ -2049,10 +2048,10 @@
       <c r="C33" s="1">
         <v>1</v>
       </c>
-      <c r="D33" s="4">
+      <c r="D33" s="2">
         <v>0.5</v>
       </c>
-      <c r="F33" s="4">
+      <c r="F33" s="2">
         <v>0.2</v>
       </c>
       <c r="H33" s="1">
@@ -2069,16 +2068,16 @@
       <c r="C34" s="1">
         <v>1</v>
       </c>
-      <c r="D34" s="4">
+      <c r="D34" s="2">
         <v>0.15</v>
       </c>
-      <c r="E34" s="4">
+      <c r="E34" s="2">
         <v>0.15</v>
       </c>
-      <c r="F34" s="4">
+      <c r="F34" s="2">
         <v>0.15</v>
       </c>
-      <c r="G34" s="4">
+      <c r="G34" s="2">
         <v>0.15</v>
       </c>
       <c r="H34" s="1">
@@ -2092,16 +2091,16 @@
       <c r="C35" s="1">
         <v>2</v>
       </c>
-      <c r="D35" s="4">
+      <c r="D35" s="2">
         <v>0.12</v>
       </c>
-      <c r="E35" s="4">
+      <c r="E35" s="2">
         <v>0.15</v>
       </c>
-      <c r="F35" s="4">
+      <c r="F35" s="2">
         <v>0.08</v>
       </c>
-      <c r="G35" s="4">
+      <c r="G35" s="2">
         <v>0.1</v>
       </c>
       <c r="H35" s="1">
@@ -2118,7 +2117,7 @@
       <c r="C36" s="1">
         <v>1</v>
       </c>
-      <c r="D36" s="4">
+      <c r="D36" s="2">
         <v>1</v>
       </c>
     </row>
@@ -2129,7 +2128,7 @@
       <c r="C37" s="1">
         <v>1</v>
       </c>
-      <c r="E37" s="4">
+      <c r="E37" s="2">
         <v>1</v>
       </c>
     </row>
@@ -2140,7 +2139,7 @@
       <c r="C38" s="1">
         <v>1</v>
       </c>
-      <c r="F38" s="4">
+      <c r="F38" s="2">
         <v>1</v>
       </c>
     </row>
@@ -2151,7 +2150,7 @@
       <c r="C39" s="1">
         <v>1</v>
       </c>
-      <c r="G39" s="4">
+      <c r="G39" s="2">
         <v>1</v>
       </c>
     </row>
@@ -2204,19 +2203,19 @@
       <c r="B45" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C45" s="8">
+      <c r="C45" s="6">
         <v>0.15</v>
       </c>
-      <c r="D45" s="5">
+      <c r="D45" s="4">
         <v>47600000</v>
       </c>
-      <c r="E45" s="6">
+      <c r="E45" s="5">
         <v>0.2</v>
       </c>
-      <c r="F45" s="5">
+      <c r="F45" s="4">
         <v>9520000</v>
       </c>
-      <c r="G45" s="4">
+      <c r="G45" s="2">
         <v>6</v>
       </c>
       <c r="H45" s="1">
@@ -2227,19 +2226,19 @@
       <c r="B46" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C46" s="8">
+      <c r="C46" s="6">
         <v>0.2</v>
       </c>
-      <c r="D46" s="5">
+      <c r="D46" s="4">
         <v>63466667</v>
       </c>
-      <c r="E46" s="6">
+      <c r="E46" s="5">
         <v>0.2</v>
       </c>
-      <c r="F46" s="5">
+      <c r="F46" s="4">
         <v>12693333.4</v>
       </c>
-      <c r="G46" s="4">
+      <c r="G46" s="2">
         <v>4.5</v>
       </c>
       <c r="H46" s="1">
@@ -2250,19 +2249,19 @@
       <c r="B47" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C47" s="8">
+      <c r="C47" s="6">
         <v>0.35</v>
       </c>
-      <c r="D47" s="5">
+      <c r="D47" s="4">
         <v>111066667</v>
       </c>
-      <c r="E47" s="6">
+      <c r="E47" s="5">
         <v>0.1</v>
       </c>
-      <c r="F47" s="5">
+      <c r="F47" s="4">
         <v>11106666.700000001</v>
       </c>
-      <c r="G47" s="4">
+      <c r="G47" s="2">
         <v>3.5</v>
       </c>
       <c r="H47" s="1">
@@ -2273,19 +2272,19 @@
       <c r="B48" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C48" s="8">
+      <c r="C48" s="6">
         <v>0.3</v>
       </c>
-      <c r="D48" s="5">
+      <c r="D48" s="4">
         <v>95200000</v>
       </c>
-      <c r="E48" s="6">
+      <c r="E48" s="5">
         <v>0.1</v>
       </c>
-      <c r="F48" s="5">
+      <c r="F48" s="4">
         <v>9520000</v>
       </c>
-      <c r="G48" s="4">
+      <c r="G48" s="2">
         <v>2.2000000000000002</v>
       </c>
       <c r="H48" s="1">
@@ -2298,34 +2297,34 @@
       </c>
     </row>
     <row r="52" spans="2:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="12" t="s">
+      <c r="B52" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C52" s="12"/>
-      <c r="D52" s="12"/>
-      <c r="E52" s="12"/>
-    </row>
-    <row r="53" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D53" s="10"/>
-      <c r="E53" s="10"/>
-      <c r="F53" s="10"/>
-      <c r="G53" s="10"/>
+      <c r="C52" s="11"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="11"/>
+    </row>
+    <row r="53" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D53" s="8"/>
+      <c r="E53" s="8"/>
+      <c r="F53" s="8"/>
+      <c r="G53" s="8"/>
     </row>
     <row r="54" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C54" s="11" t="s">
+      <c r="C54" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D54" s="11"/>
-      <c r="E54" s="11"/>
+      <c r="D54" s="10"/>
+      <c r="E54" s="10"/>
     </row>
     <row r="55" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C55" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D55" s="4" t="s">
+      <c r="D55" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E55" s="4" t="s">
+      <c r="E55" s="2" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2341,10 +2340,10 @@
       <c r="C57" s="1">
         <v>600</v>
       </c>
-      <c r="D57" s="4">
+      <c r="D57" s="2">
         <v>600</v>
       </c>
-      <c r="E57" s="4">
+      <c r="E57" s="2">
         <v>600</v>
       </c>
     </row>
@@ -2355,10 +2354,10 @@
       <c r="C58" s="1">
         <v>600</v>
       </c>
-      <c r="D58" s="4">
+      <c r="D58" s="2">
         <v>600</v>
       </c>
-      <c r="E58" s="4">
+      <c r="E58" s="2">
         <v>600</v>
       </c>
     </row>
@@ -2369,10 +2368,10 @@
       <c r="C59" s="1">
         <v>600</v>
       </c>
-      <c r="D59" s="4">
+      <c r="D59" s="2">
         <v>600</v>
       </c>
-      <c r="E59" s="4">
+      <c r="E59" s="2">
         <v>600</v>
       </c>
     </row>
@@ -2388,10 +2387,10 @@
       <c r="C61" s="1">
         <v>1600</v>
       </c>
-      <c r="D61" s="4">
+      <c r="D61" s="2">
         <v>1500</v>
       </c>
-      <c r="E61" s="4">
+      <c r="E61" s="2">
         <v>1800</v>
       </c>
     </row>
@@ -2402,10 +2401,10 @@
       <c r="C62" s="1">
         <v>1839.9999999999998</v>
       </c>
-      <c r="D62" s="4">
+      <c r="D62" s="2">
         <v>1724.9999999999998</v>
       </c>
-      <c r="E62" s="4">
+      <c r="E62" s="2">
         <v>2070</v>
       </c>
     </row>
@@ -2416,10 +2415,10 @@
       <c r="C63" s="1">
         <v>1839.9999999999998</v>
       </c>
-      <c r="D63" s="4">
+      <c r="D63" s="2">
         <v>1724.9999999999998</v>
       </c>
-      <c r="E63" s="4">
+      <c r="E63" s="2">
         <v>2070</v>
       </c>
     </row>
@@ -2438,39 +2437,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A5637ED-8D1B-4849-B877-4C79A797D7C0}">
   <dimension ref="A1:H291"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A263" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M280" sqref="M280"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.88671875" customWidth="1"/>
     <col min="5" max="5" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="14" customFormat="1" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:8" s="9" customFormat="1" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="9" t="s">
         <v>347</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="9" t="s">
         <v>55</v>
       </c>
     </row>
@@ -10017,4 +10016,1000 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{267E78CF-C385-4A01-A1A0-0ADB97B6A8A6}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D3" s="2">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2">
+        <v>2.875</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="E4" s="2">
+        <v>2.375</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1.8250000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.27</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1.5449999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A2C8130-8429-4D19-980D-21B56E64C626}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="F2" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1.2E-2</v>
+      </c>
+      <c r="E3" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="F3" s="2">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="F4" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1.2E-2</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="F5" s="2">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="F6" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1.2E-2</v>
+      </c>
+      <c r="E7" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="F7" s="2">
+        <v>2E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{106E24B4-FA99-4C05-9C9C-3DC382398A8C}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.92</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.91</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.93</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.94</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E3C409F-772B-49A7-B6E3-401FF4E0BC50}">
+  <dimension ref="A1:H16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1">
+        <v>2</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2">
+        <v>1</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2">
+        <v>1</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="1">
+        <v>1</v>
+      </c>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A38DDE21-5AD8-430F-98F0-781DE3D1DF21}">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6">
+        <v>0.15</v>
+      </c>
+      <c r="C2" s="4">
+        <v>47600000</v>
+      </c>
+      <c r="D2" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="E2" s="4">
+        <v>9520000</v>
+      </c>
+      <c r="F2" s="2">
+        <v>6</v>
+      </c>
+      <c r="G2" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="C3" s="4">
+        <v>63466667</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="E3" s="4">
+        <v>12693333.4</v>
+      </c>
+      <c r="F3" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="G3" s="1">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6">
+        <v>0.35</v>
+      </c>
+      <c r="C4" s="4">
+        <v>111066667</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="E4" s="4">
+        <v>11106666.700000001</v>
+      </c>
+      <c r="F4" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="G4" s="1">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="C5" s="4">
+        <v>95200000</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="E5" s="4">
+        <v>9520000</v>
+      </c>
+      <c r="F5" s="2">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{568BCC57-FC4A-4B13-BECD-8A887D7D049D}">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1">
+        <v>600</v>
+      </c>
+      <c r="C4" s="2">
+        <v>600</v>
+      </c>
+      <c r="D4" s="2">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1">
+        <v>600</v>
+      </c>
+      <c r="C5" s="2">
+        <v>600</v>
+      </c>
+      <c r="D5" s="2">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1">
+        <v>600</v>
+      </c>
+      <c r="C6" s="2">
+        <v>600</v>
+      </c>
+      <c r="D6" s="2">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1600</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1500</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1839.9999999999998</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1724.9999999999998</v>
+      </c>
+      <c r="D9" s="2">
+        <v>2070</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1839.9999999999998</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1724.9999999999998</v>
+      </c>
+      <c r="D10" s="2">
+        <v>2070</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
ecc calidad sin lluvia lista
</commit_message>
<xml_diff>
--- a/info-vinos_2023_v2.xlsx
+++ b/info-vinos_2023_v2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\crisiturriaga\Proyecto-capstone\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uccl0-my.sharepoint.com/personal/martinramirez_uc_cl/Documents/Documents/UC/8vo semestre/Capstone/Proyecto/Proyecto-capstone/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA229CE-E846-42CE-A9FF-97855FD6D06C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="13_ncr:1_{7EA229CE-E846-42CE-A9FF-97855FD6D06C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9ABFA6A-6F7F-4498-B1C3-08099CC4B359}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{9FE83E1C-AE4E-4FF0-90CF-2F394FA28AC8}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{9FE83E1C-AE4E-4FF0-90CF-2F394FA28AC8}"/>
   </bookViews>
   <sheets>
     <sheet name="info 2023" sheetId="9" r:id="rId1"/>
@@ -1091,8 +1091,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -1149,7 +1149,7 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
@@ -1163,7 +1163,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
@@ -1508,31 +1508,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{988F2DAE-07FB-46B3-A14C-238B483C364F}">
   <dimension ref="B2:M63"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54:E63"/>
+    <sheetView tabSelected="1" zoomScale="78" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18:F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="23.77734375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.86328125" style="1"/>
+    <col min="2" max="2" width="23.796875" style="1" customWidth="1"/>
     <col min="3" max="3" width="13" style="1" customWidth="1"/>
     <col min="4" max="4" width="15.33203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="17.109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="12.77734375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="12.88671875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="17.1328125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.796875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="12.86328125" style="2" customWidth="1"/>
     <col min="8" max="8" width="11" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.88671875" style="1"/>
-    <col min="10" max="10" width="11.5546875" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="1"/>
+    <col min="9" max="9" width="8.86328125" style="1"/>
+    <col min="10" max="10" width="11.53125" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.86328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.45">
       <c r="C2" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B3" s="2" t="s">
         <v>35</v>
       </c>
@@ -1549,7 +1549,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -1566,7 +1566,7 @@
         <v>2.875</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
@@ -1583,7 +1583,7 @@
         <v>2.375</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -1600,7 +1600,7 @@
         <v>1.8250000000000002</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
@@ -1617,7 +1617,7 @@
         <v>1.5449999999999999</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B10" s="1" t="s">
         <v>0</v>
       </c>
@@ -1637,7 +1637,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B11" s="1" t="s">
         <v>21</v>
       </c>
@@ -1657,7 +1657,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B12" s="1" t="s">
         <v>22</v>
       </c>
@@ -1677,7 +1677,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B13" s="1" t="s">
         <v>23</v>
       </c>
@@ -1697,7 +1697,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B14" s="1" t="s">
         <v>24</v>
       </c>
@@ -1717,7 +1717,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B15" s="1" t="s">
         <v>25</v>
       </c>
@@ -1737,7 +1737,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B16" s="1" t="s">
         <v>26</v>
       </c>
@@ -1757,7 +1757,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="18" spans="2:13" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:13" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B18" s="1" t="s">
         <v>0</v>
       </c>
@@ -1774,7 +1774,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B19" s="1" t="s">
         <v>21</v>
       </c>
@@ -1799,7 +1799,7 @@
       <c r="L19" s="12"/>
       <c r="M19" s="12"/>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B20" s="1" t="s">
         <v>22</v>
       </c>
@@ -1822,7 +1822,7 @@
       <c r="L20" s="12"/>
       <c r="M20" s="12"/>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B21" s="1" t="s">
         <v>23</v>
       </c>
@@ -1845,7 +1845,7 @@
       <c r="L21" s="12"/>
       <c r="M21" s="12"/>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B22" s="1" t="s">
         <v>24</v>
       </c>
@@ -1868,7 +1868,7 @@
       <c r="L22" s="12"/>
       <c r="M22" s="12"/>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B23" s="1" t="s">
         <v>25</v>
       </c>
@@ -1891,7 +1891,7 @@
       <c r="L23" s="12"/>
       <c r="M23" s="12"/>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B24" s="1" t="s">
         <v>26</v>
       </c>
@@ -1908,7 +1908,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.45">
       <c r="D26" s="10" t="s">
         <v>54</v>
       </c>
@@ -1918,7 +1918,7 @@
       <c r="H26" s="10"/>
       <c r="I26" s="10"/>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B27" s="1" t="s">
         <v>10</v>
       </c>
@@ -1944,7 +1944,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B28" s="1" t="s">
         <v>30</v>
       </c>
@@ -1964,7 +1964,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.45">
       <c r="C29" s="1">
         <v>2</v>
       </c>
@@ -1981,7 +1981,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B30" s="1" t="s">
         <v>31</v>
       </c>
@@ -2004,7 +2004,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.45">
       <c r="C31" s="1">
         <v>2</v>
       </c>
@@ -2024,7 +2024,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.45">
       <c r="C32" s="1">
         <v>3</v>
       </c>
@@ -2041,7 +2041,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B33" s="1" t="s">
         <v>32</v>
       </c>
@@ -2061,7 +2061,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B34" s="1" t="s">
         <v>33</v>
       </c>
@@ -2087,7 +2087,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.45">
       <c r="C35" s="1">
         <v>2</v>
       </c>
@@ -2110,7 +2110,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B36" s="1" t="s">
         <v>21</v>
       </c>
@@ -2121,7 +2121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B37" s="1" t="s">
         <v>22</v>
       </c>
@@ -2132,7 +2132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B38" s="1" t="s">
         <v>23</v>
       </c>
@@ -2143,7 +2143,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B39" s="1" t="s">
         <v>24</v>
       </c>
@@ -2154,7 +2154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B40" s="1" t="s">
         <v>25</v>
       </c>
@@ -2165,7 +2165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B41" s="1" t="s">
         <v>26</v>
       </c>
@@ -2176,7 +2176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="2:9" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:9" s="3" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B44" s="3" t="s">
         <v>35</v>
       </c>
@@ -2199,7 +2199,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B45" s="1" t="s">
         <v>1</v>
       </c>
@@ -2222,7 +2222,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B46" s="1" t="s">
         <v>2</v>
       </c>
@@ -2245,7 +2245,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B47" s="1" t="s">
         <v>3</v>
       </c>
@@ -2268,7 +2268,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B48" s="1" t="s">
         <v>4</v>
       </c>
@@ -2291,12 +2291,12 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B51" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="52" spans="2:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B52" s="11" t="s">
         <v>41</v>
       </c>
@@ -2304,20 +2304,20 @@
       <c r="D52" s="11"/>
       <c r="E52" s="11"/>
     </row>
-    <row r="53" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.45">
       <c r="D53" s="8"/>
       <c r="E53" s="8"/>
       <c r="F53" s="8"/>
       <c r="G53" s="8"/>
     </row>
-    <row r="54" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C54" s="10" t="s">
         <v>43</v>
       </c>
       <c r="D54" s="10"/>
       <c r="E54" s="10"/>
     </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:7" x14ac:dyDescent="0.45">
       <c r="C55" s="1" t="s">
         <v>12</v>
       </c>
@@ -2328,12 +2328,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="56" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B56" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B57" s="1" t="s">
         <v>15</v>
       </c>
@@ -2347,7 +2347,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B58" s="1" t="s">
         <v>16</v>
       </c>
@@ -2361,7 +2361,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B59" s="1" t="s">
         <v>17</v>
       </c>
@@ -2375,12 +2375,12 @@
         <v>600</v>
       </c>
     </row>
-    <row r="60" spans="2:7" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:7" ht="29.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B60" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B61" s="1" t="s">
         <v>15</v>
       </c>
@@ -2394,7 +2394,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B62" s="1" t="s">
         <v>16</v>
       </c>
@@ -2408,7 +2408,7 @@
         <v>2070</v>
       </c>
     </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B63" s="1" t="s">
         <v>17</v>
       </c>
@@ -2441,13 +2441,13 @@
       <selection activeCell="M280" sqref="M280"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" customWidth="1"/>
-    <col min="5" max="5" width="12.88671875" customWidth="1"/>
+    <col min="1" max="1" width="10.86328125" customWidth="1"/>
+    <col min="5" max="5" width="12.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="9" customFormat="1" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="9" customFormat="1" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="9" t="s">
         <v>7</v>
       </c>
@@ -2473,7 +2473,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>56</v>
       </c>
@@ -2499,7 +2499,7 @@
         <v>0.25700000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>57</v>
       </c>
@@ -2525,7 +2525,7 @@
         <v>0.26900000000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -2551,7 +2551,7 @@
         <v>0.36199999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>59</v>
       </c>
@@ -2577,7 +2577,7 @@
         <v>0.27600000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>60</v>
       </c>
@@ -2603,7 +2603,7 @@
         <v>0.34799999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>61</v>
       </c>
@@ -2629,7 +2629,7 @@
         <v>0.57899999999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>62</v>
       </c>
@@ -2655,7 +2655,7 @@
         <v>0.79500000000000004</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>63</v>
       </c>
@@ -2681,7 +2681,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>64</v>
       </c>
@@ -2707,7 +2707,7 @@
         <v>0.52800000000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>65</v>
       </c>
@@ -2733,7 +2733,7 @@
         <v>0.80600000000000005</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>66</v>
       </c>
@@ -2759,7 +2759,7 @@
         <v>0.55700000000000005</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>67</v>
       </c>
@@ -2785,7 +2785,7 @@
         <v>0.51600000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>68</v>
       </c>
@@ -2811,7 +2811,7 @@
         <v>0.81100000000000005</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>69</v>
       </c>
@@ -2837,7 +2837,7 @@
         <v>0.41599999999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>70</v>
       </c>
@@ -2863,7 +2863,7 @@
         <v>0.55400000000000005</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>71</v>
       </c>
@@ -2889,7 +2889,7 @@
         <v>0.36099999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>72</v>
       </c>
@@ -2915,7 +2915,7 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>73</v>
       </c>
@@ -2941,7 +2941,7 @@
         <v>0.40699999999999997</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>74</v>
       </c>
@@ -2967,7 +2967,7 @@
         <v>0.41299999999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>75</v>
       </c>
@@ -2993,7 +2993,7 @@
         <v>0.27400000000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>76</v>
       </c>
@@ -3019,7 +3019,7 @@
         <v>0.82799999999999996</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>77</v>
       </c>
@@ -3045,7 +3045,7 @@
         <v>0.55400000000000005</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>78</v>
       </c>
@@ -3071,7 +3071,7 @@
         <v>0.60099999999999998</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>79</v>
       </c>
@@ -3097,7 +3097,7 @@
         <v>0.80800000000000005</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>80</v>
       </c>
@@ -3123,7 +3123,7 @@
         <v>0.58799999999999997</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>81</v>
       </c>
@@ -3149,7 +3149,7 @@
         <v>0.35599999999999998</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>82</v>
       </c>
@@ -3175,7 +3175,7 @@
         <v>0.36099999999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>83</v>
       </c>
@@ -3201,7 +3201,7 @@
         <v>0.59599999999999997</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>84</v>
       </c>
@@ -3227,7 +3227,7 @@
         <v>0.54900000000000004</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>85</v>
       </c>
@@ -3253,7 +3253,7 @@
         <v>0.27300000000000002</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>86</v>
       </c>
@@ -3279,7 +3279,7 @@
         <v>0.54400000000000004</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>87</v>
       </c>
@@ -3305,7 +3305,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>88</v>
       </c>
@@ -3331,7 +3331,7 @@
         <v>0.34399999999999997</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>89</v>
       </c>
@@ -3357,7 +3357,7 @@
         <v>0.40300000000000002</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>90</v>
       </c>
@@ -3383,7 +3383,7 @@
         <v>0.82799999999999996</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>91</v>
       </c>
@@ -3409,7 +3409,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>92</v>
       </c>
@@ -3435,7 +3435,7 @@
         <v>0.34499999999999997</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>93</v>
       </c>
@@ -3461,7 +3461,7 @@
         <v>0.54400000000000004</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>94</v>
       </c>
@@ -3487,7 +3487,7 @@
         <v>0.35699999999999998</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>95</v>
       </c>
@@ -3513,7 +3513,7 @@
         <v>0.53300000000000003</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>96</v>
       </c>
@@ -3539,7 +3539,7 @@
         <v>0.54400000000000004</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>97</v>
       </c>
@@ -3565,7 +3565,7 @@
         <v>0.25900000000000001</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>98</v>
       </c>
@@ -3591,7 +3591,7 @@
         <v>0.53100000000000003</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>99</v>
       </c>
@@ -3617,7 +3617,7 @@
         <v>0.41199999999999998</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>100</v>
       </c>
@@ -3643,7 +3643,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>101</v>
       </c>
@@ -3669,7 +3669,7 @@
         <v>0.26700000000000002</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>102</v>
       </c>
@@ -3695,7 +3695,7 @@
         <v>0.39600000000000002</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>103</v>
       </c>
@@ -3721,7 +3721,7 @@
         <v>0.54100000000000004</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>104</v>
       </c>
@@ -3747,7 +3747,7 @@
         <v>0.83099999999999996</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>105</v>
       </c>
@@ -3773,7 +3773,7 @@
         <v>0.78100000000000003</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>106</v>
       </c>
@@ -3799,7 +3799,7 @@
         <v>0.52600000000000002</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>107</v>
       </c>
@@ -3825,7 +3825,7 @@
         <v>0.40600000000000003</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>108</v>
       </c>
@@ -3851,7 +3851,7 @@
         <v>0.34499999999999997</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>109</v>
       </c>
@@ -3877,7 +3877,7 @@
         <v>0.39400000000000002</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>110</v>
       </c>
@@ -3903,7 +3903,7 @@
         <v>0.40799999999999997</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>111</v>
       </c>
@@ -3929,7 +3929,7 @@
         <v>0.39500000000000002</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>112</v>
       </c>
@@ -3955,7 +3955,7 @@
         <v>0.79800000000000004</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>113</v>
       </c>
@@ -3981,7 +3981,7 @@
         <v>0.27200000000000002</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>114</v>
       </c>
@@ -4007,7 +4007,7 @@
         <v>0.82899999999999996</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>115</v>
       </c>
@@ -4033,7 +4033,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>116</v>
       </c>
@@ -4059,7 +4059,7 @@
         <v>0.51300000000000001</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>117</v>
       </c>
@@ -4085,7 +4085,7 @@
         <v>0.55100000000000005</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>118</v>
       </c>
@@ -4111,7 +4111,7 @@
         <v>0.58799999999999997</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>119</v>
       </c>
@@ -4137,7 +4137,7 @@
         <v>0.41599999999999998</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>120</v>
       </c>
@@ -4163,7 +4163,7 @@
         <v>0.58399999999999996</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>121</v>
       </c>
@@ -4189,7 +4189,7 @@
         <v>0.60199999999999998</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>122</v>
       </c>
@@ -4215,7 +4215,7 @@
         <v>0.59099999999999997</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>123</v>
       </c>
@@ -4241,7 +4241,7 @@
         <v>0.55500000000000005</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>124</v>
       </c>
@@ -4267,7 +4267,7 @@
         <v>0.54800000000000004</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>125</v>
       </c>
@@ -4293,7 +4293,7 @@
         <v>0.82199999999999995</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>126</v>
       </c>
@@ -4319,7 +4319,7 @@
         <v>0.81699999999999995</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>127</v>
       </c>
@@ -4345,7 +4345,7 @@
         <v>0.52800000000000002</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>128</v>
       </c>
@@ -4371,7 +4371,7 @@
         <v>0.39200000000000002</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>129</v>
       </c>
@@ -4397,7 +4397,7 @@
         <v>0.41699999999999998</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>130</v>
       </c>
@@ -4423,7 +4423,7 @@
         <v>0.41499999999999998</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>131</v>
       </c>
@@ -4449,7 +4449,7 @@
         <v>0.41499999999999998</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>132</v>
       </c>
@@ -4475,7 +4475,7 @@
         <v>0.40400000000000003</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>133</v>
       </c>
@@ -4501,7 +4501,7 @@
         <v>0.80100000000000005</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>134</v>
       </c>
@@ -4527,7 +4527,7 @@
         <v>0.83399999999999996</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
         <v>135</v>
       </c>
@@ -4553,7 +4553,7 @@
         <v>0.77</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
         <v>136</v>
       </c>
@@ -4579,7 +4579,7 @@
         <v>0.79500000000000004</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
         <v>137</v>
       </c>
@@ -4605,7 +4605,7 @@
         <v>0.40899999999999997</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
         <v>138</v>
       </c>
@@ -4631,7 +4631,7 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>139</v>
       </c>
@@ -4657,7 +4657,7 @@
         <v>0.53600000000000003</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
         <v>140</v>
       </c>
@@ -4683,7 +4683,7 @@
         <v>0.26500000000000001</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
         <v>141</v>
       </c>
@@ -4709,7 +4709,7 @@
         <v>0.83299999999999996</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
         <v>142</v>
       </c>
@@ -4735,7 +4735,7 @@
         <v>0.60599999999999998</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
         <v>143</v>
       </c>
@@ -4761,7 +4761,7 @@
         <v>0.53800000000000003</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
         <v>144</v>
       </c>
@@ -4787,7 +4787,7 @@
         <v>0.35599999999999998</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
         <v>145</v>
       </c>
@@ -4813,7 +4813,7 @@
         <v>0.35699999999999998</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>146</v>
       </c>
@@ -4839,7 +4839,7 @@
         <v>0.57599999999999996</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
         <v>147</v>
       </c>
@@ -4865,7 +4865,7 @@
         <v>0.83199999999999996</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
         <v>148</v>
       </c>
@@ -4891,7 +4891,7 @@
         <v>0.54400000000000004</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
         <v>149</v>
       </c>
@@ -4917,7 +4917,7 @@
         <v>0.35599999999999998</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
         <v>150</v>
       </c>
@@ -4943,7 +4943,7 @@
         <v>0.78700000000000003</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
         <v>151</v>
       </c>
@@ -4969,7 +4969,7 @@
         <v>0.76400000000000001</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
         <v>152</v>
       </c>
@@ -4995,7 +4995,7 @@
         <v>0.34799999999999998</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
         <v>153</v>
       </c>
@@ -5021,7 +5021,7 @@
         <v>0.27800000000000002</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
         <v>154</v>
       </c>
@@ -5047,7 +5047,7 @@
         <v>0.41499999999999998</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
         <v>155</v>
       </c>
@@ -5073,7 +5073,7 @@
         <v>0.33800000000000002</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
         <v>156</v>
       </c>
@@ -5099,7 +5099,7 @@
         <v>0.40600000000000003</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
         <v>157</v>
       </c>
@@ -5125,7 +5125,7 @@
         <v>0.81799999999999995</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
         <v>158</v>
       </c>
@@ -5151,7 +5151,7 @@
         <v>0.40500000000000003</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
         <v>159</v>
       </c>
@@ -5177,7 +5177,7 @@
         <v>0.26400000000000001</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
         <v>160</v>
       </c>
@@ -5203,7 +5203,7 @@
         <v>0.40799999999999997</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
         <v>161</v>
       </c>
@@ -5229,7 +5229,7 @@
         <v>0.55600000000000005</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
         <v>162</v>
       </c>
@@ -5255,7 +5255,7 @@
         <v>0.52400000000000002</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
         <v>163</v>
       </c>
@@ -5281,7 +5281,7 @@
         <v>0.27700000000000002</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A110" t="s">
         <v>164</v>
       </c>
@@ -5307,7 +5307,7 @@
         <v>0.27700000000000002</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
         <v>165</v>
       </c>
@@ -5333,7 +5333,7 @@
         <v>0.60099999999999998</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A112" t="s">
         <v>166</v>
       </c>
@@ -5359,7 +5359,7 @@
         <v>0.57299999999999995</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
         <v>167</v>
       </c>
@@ -5385,7 +5385,7 @@
         <v>0.55400000000000005</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A114" t="s">
         <v>168</v>
       </c>
@@ -5411,7 +5411,7 @@
         <v>0.55400000000000005</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A115" t="s">
         <v>169</v>
       </c>
@@ -5437,7 +5437,7 @@
         <v>0.61</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
         <v>170</v>
       </c>
@@ -5463,7 +5463,7 @@
         <v>0.60899999999999999</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A117" t="s">
         <v>171</v>
       </c>
@@ -5489,7 +5489,7 @@
         <v>0.59199999999999997</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A118" t="s">
         <v>172</v>
       </c>
@@ -5515,7 +5515,7 @@
         <v>0.51900000000000002</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A119" t="s">
         <v>173</v>
       </c>
@@ -5541,7 +5541,7 @@
         <v>0.34399999999999997</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A120" t="s">
         <v>174</v>
       </c>
@@ -5567,7 +5567,7 @@
         <v>0.36099999999999999</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A121" t="s">
         <v>175</v>
       </c>
@@ -5593,7 +5593,7 @@
         <v>0.60499999999999998</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A122" t="s">
         <v>176</v>
       </c>
@@ -5619,7 +5619,7 @@
         <v>0.82299999999999995</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A123" t="s">
         <v>177</v>
       </c>
@@ -5645,7 +5645,7 @@
         <v>0.35799999999999998</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A124" t="s">
         <v>178</v>
       </c>
@@ -5671,7 +5671,7 @@
         <v>0.55700000000000005</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A125" t="s">
         <v>179</v>
       </c>
@@ -5697,7 +5697,7 @@
         <v>0.35899999999999999</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A126" t="s">
         <v>180</v>
       </c>
@@ -5723,7 +5723,7 @@
         <v>0.27200000000000002</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A127" t="s">
         <v>181</v>
       </c>
@@ -5749,7 +5749,7 @@
         <v>0.83099999999999996</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A128" t="s">
         <v>182</v>
       </c>
@@ -5775,7 +5775,7 @@
         <v>0.81299999999999994</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A129" t="s">
         <v>183</v>
       </c>
@@ -5801,7 +5801,7 @@
         <v>0.54100000000000004</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A130" t="s">
         <v>184</v>
       </c>
@@ -5827,7 +5827,7 @@
         <v>0.55600000000000005</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A131" t="s">
         <v>185</v>
       </c>
@@ -5853,7 +5853,7 @@
         <v>0.60899999999999999</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A132" t="s">
         <v>186</v>
       </c>
@@ -5879,7 +5879,7 @@
         <v>0.35099999999999998</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A133" t="s">
         <v>187</v>
       </c>
@@ -5905,7 +5905,7 @@
         <v>0.41399999999999998</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A134" t="s">
         <v>188</v>
       </c>
@@ -5931,7 +5931,7 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A135" t="s">
         <v>189</v>
       </c>
@@ -5957,7 +5957,7 @@
         <v>0.27300000000000002</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A136" t="s">
         <v>190</v>
       </c>
@@ -5983,7 +5983,7 @@
         <v>0.27300000000000002</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A137" t="s">
         <v>191</v>
       </c>
@@ -6009,7 +6009,7 @@
         <v>0.59099999999999997</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A138" t="s">
         <v>192</v>
       </c>
@@ -6035,7 +6035,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A139" t="s">
         <v>193</v>
       </c>
@@ -6061,7 +6061,7 @@
         <v>0.53600000000000003</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A140" t="s">
         <v>194</v>
       </c>
@@ -6087,7 +6087,7 @@
         <v>0.35799999999999998</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A141" t="s">
         <v>195</v>
       </c>
@@ -6113,7 +6113,7 @@
         <v>0.60699999999999998</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A142" t="s">
         <v>196</v>
       </c>
@@ -6139,7 +6139,7 @@
         <v>0.83499999999999996</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A143" t="s">
         <v>197</v>
       </c>
@@ -6165,7 +6165,7 @@
         <v>0.81399999999999995</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A144" t="s">
         <v>198</v>
       </c>
@@ -6191,7 +6191,7 @@
         <v>0.39900000000000002</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A145" t="s">
         <v>199</v>
       </c>
@@ -6217,7 +6217,7 @@
         <v>0.27100000000000002</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A146" t="s">
         <v>200</v>
       </c>
@@ -6243,7 +6243,7 @@
         <v>0.40400000000000003</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A147" t="s">
         <v>201</v>
       </c>
@@ -6269,7 +6269,7 @@
         <v>0.81399999999999995</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A148" t="s">
         <v>202</v>
       </c>
@@ -6295,7 +6295,7 @@
         <v>0.55600000000000005</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A149" t="s">
         <v>203</v>
       </c>
@@ -6321,7 +6321,7 @@
         <v>0.35099999999999998</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A150" t="s">
         <v>204</v>
       </c>
@@ -6347,7 +6347,7 @@
         <v>0.79800000000000004</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A151" t="s">
         <v>205</v>
       </c>
@@ -6373,7 +6373,7 @@
         <v>0.34300000000000003</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A152" t="s">
         <v>206</v>
       </c>
@@ -6399,7 +6399,7 @@
         <v>0.35599999999999998</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A153" t="s">
         <v>207</v>
       </c>
@@ -6425,7 +6425,7 @@
         <v>0.80200000000000005</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A154" t="s">
         <v>208</v>
       </c>
@@ -6451,7 +6451,7 @@
         <v>0.82199999999999995</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A155" t="s">
         <v>209</v>
       </c>
@@ -6477,7 +6477,7 @@
         <v>0.60799999999999998</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A156" t="s">
         <v>210</v>
       </c>
@@ -6503,7 +6503,7 @@
         <v>0.27200000000000002</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A157" t="s">
         <v>211</v>
       </c>
@@ -6529,7 +6529,7 @@
         <v>0.26600000000000001</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A158" t="s">
         <v>212</v>
       </c>
@@ -6555,7 +6555,7 @@
         <v>0.39300000000000002</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A159" t="s">
         <v>213</v>
       </c>
@@ -6581,7 +6581,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A160" t="s">
         <v>214</v>
       </c>
@@ -6607,7 +6607,7 @@
         <v>0.83399999999999996</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A161" t="s">
         <v>215</v>
       </c>
@@ -6633,7 +6633,7 @@
         <v>0.55200000000000005</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A162" t="s">
         <v>216</v>
       </c>
@@ -6659,7 +6659,7 @@
         <v>0.34799999999999998</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A163" t="s">
         <v>217</v>
       </c>
@@ -6685,7 +6685,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A164" t="s">
         <v>218</v>
       </c>
@@ -6711,7 +6711,7 @@
         <v>0.54700000000000004</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A165" t="s">
         <v>219</v>
       </c>
@@ -6737,7 +6737,7 @@
         <v>0.82899999999999996</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A166" t="s">
         <v>220</v>
       </c>
@@ -6763,7 +6763,7 @@
         <v>0.27200000000000002</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A167" t="s">
         <v>221</v>
       </c>
@@ -6789,7 +6789,7 @@
         <v>0.26700000000000002</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A168" t="s">
         <v>222</v>
       </c>
@@ -6815,7 +6815,7 @@
         <v>0.27400000000000002</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A169" t="s">
         <v>223</v>
       </c>
@@ -6841,7 +6841,7 @@
         <v>0.41199999999999998</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A170" t="s">
         <v>224</v>
       </c>
@@ -6867,7 +6867,7 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A171" t="s">
         <v>225</v>
       </c>
@@ -6893,7 +6893,7 @@
         <v>0.82899999999999996</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A172" t="s">
         <v>226</v>
       </c>
@@ -6919,7 +6919,7 @@
         <v>0.58799999999999997</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A173" t="s">
         <v>227</v>
       </c>
@@ -6945,7 +6945,7 @@
         <v>0.55600000000000005</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A174" t="s">
         <v>228</v>
       </c>
@@ -6971,7 +6971,7 @@
         <v>0.55200000000000005</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A175" t="s">
         <v>229</v>
       </c>
@@ -6997,7 +6997,7 @@
         <v>0.41399999999999998</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A176" t="s">
         <v>230</v>
       </c>
@@ -7023,7 +7023,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A177" t="s">
         <v>231</v>
       </c>
@@ -7049,7 +7049,7 @@
         <v>0.55700000000000005</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A178" t="s">
         <v>232</v>
       </c>
@@ -7075,7 +7075,7 @@
         <v>0.58899999999999997</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A179" t="s">
         <v>233</v>
       </c>
@@ -7101,7 +7101,7 @@
         <v>0.34599999999999997</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A180" t="s">
         <v>234</v>
       </c>
@@ -7127,7 +7127,7 @@
         <v>0.26400000000000001</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A181" t="s">
         <v>235</v>
       </c>
@@ -7153,7 +7153,7 @@
         <v>0.41599999999999998</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A182" t="s">
         <v>236</v>
       </c>
@@ -7179,7 +7179,7 @@
         <v>0.27400000000000002</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A183" t="s">
         <v>237</v>
       </c>
@@ -7205,7 +7205,7 @@
         <v>0.40300000000000002</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A184" t="s">
         <v>238</v>
       </c>
@@ -7231,7 +7231,7 @@
         <v>0.81799999999999995</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A185" t="s">
         <v>239</v>
       </c>
@@ -7257,7 +7257,7 @@
         <v>0.54200000000000004</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A186" t="s">
         <v>240</v>
       </c>
@@ -7283,7 +7283,7 @@
         <v>0.35699999999999998</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A187" t="s">
         <v>241</v>
       </c>
@@ -7309,7 +7309,7 @@
         <v>0.79200000000000004</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A188" t="s">
         <v>242</v>
       </c>
@@ -7335,7 +7335,7 @@
         <v>0.40100000000000002</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A189" t="s">
         <v>243</v>
       </c>
@@ -7361,7 +7361,7 @@
         <v>0.41799999999999998</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A190" t="s">
         <v>244</v>
       </c>
@@ -7387,7 +7387,7 @@
         <v>0.27700000000000002</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A191" t="s">
         <v>245</v>
       </c>
@@ -7413,7 +7413,7 @@
         <v>0.83199999999999996</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A192" t="s">
         <v>246</v>
       </c>
@@ -7439,7 +7439,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A193" t="s">
         <v>247</v>
       </c>
@@ -7465,7 +7465,7 @@
         <v>0.54800000000000004</v>
       </c>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A194" t="s">
         <v>248</v>
       </c>
@@ -7491,7 +7491,7 @@
         <v>0.35899999999999999</v>
       </c>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A195" t="s">
         <v>249</v>
       </c>
@@ -7517,7 +7517,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A196" t="s">
         <v>250</v>
       </c>
@@ -7543,7 +7543,7 @@
         <v>0.78700000000000003</v>
       </c>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A197" t="s">
         <v>251</v>
       </c>
@@ -7569,7 +7569,7 @@
         <v>0.41599999999999998</v>
       </c>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A198" t="s">
         <v>252</v>
       </c>
@@ -7595,7 +7595,7 @@
         <v>0.53900000000000003</v>
       </c>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A199" t="s">
         <v>253</v>
       </c>
@@ -7621,7 +7621,7 @@
         <v>0.60699999999999998</v>
       </c>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A200" t="s">
         <v>254</v>
       </c>
@@ -7647,7 +7647,7 @@
         <v>0.81399999999999995</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A201" t="s">
         <v>255</v>
       </c>
@@ -7673,7 +7673,7 @@
         <v>0.82799999999999996</v>
       </c>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A202" t="s">
         <v>256</v>
       </c>
@@ -7699,7 +7699,7 @@
         <v>0.53400000000000003</v>
       </c>
     </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A203" t="s">
         <v>257</v>
       </c>
@@ -7725,7 +7725,7 @@
         <v>0.56799999999999995</v>
       </c>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A204" t="s">
         <v>258</v>
       </c>
@@ -7751,7 +7751,7 @@
         <v>0.60699999999999998</v>
       </c>
     </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A205" t="s">
         <v>259</v>
       </c>
@@ -7777,7 +7777,7 @@
         <v>0.41399999999999998</v>
       </c>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A206" t="s">
         <v>260</v>
       </c>
@@ -7803,7 +7803,7 @@
         <v>0.40300000000000002</v>
       </c>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A207" t="s">
         <v>261</v>
       </c>
@@ -7829,7 +7829,7 @@
         <v>0.60799999999999998</v>
       </c>
     </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A208" t="s">
         <v>262</v>
       </c>
@@ -7855,7 +7855,7 @@
         <v>0.80200000000000005</v>
       </c>
     </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A209" t="s">
         <v>263</v>
       </c>
@@ -7881,7 +7881,7 @@
         <v>0.40799999999999997</v>
       </c>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A210" t="s">
         <v>264</v>
       </c>
@@ -7907,7 +7907,7 @@
         <v>0.82899999999999996</v>
       </c>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A211" t="s">
         <v>265</v>
       </c>
@@ -7933,7 +7933,7 @@
         <v>0.27200000000000002</v>
       </c>
     </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A212" t="s">
         <v>266</v>
       </c>
@@ -7959,7 +7959,7 @@
         <v>0.83399999999999996</v>
       </c>
     </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A213" t="s">
         <v>267</v>
       </c>
@@ -7985,7 +7985,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A214" t="s">
         <v>268</v>
       </c>
@@ -8011,7 +8011,7 @@
         <v>0.27800000000000002</v>
       </c>
     </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A215" t="s">
         <v>269</v>
       </c>
@@ -8037,7 +8037,7 @@
         <v>0.51</v>
       </c>
     </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A216" t="s">
         <v>270</v>
       </c>
@@ -8063,7 +8063,7 @@
         <v>0.35199999999999998</v>
       </c>
     </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A217" t="s">
         <v>271</v>
       </c>
@@ -8089,7 +8089,7 @@
         <v>0.41299999999999998</v>
       </c>
     </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A218" t="s">
         <v>272</v>
       </c>
@@ -8115,7 +8115,7 @@
         <v>0.59499999999999997</v>
       </c>
     </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A219" t="s">
         <v>273</v>
       </c>
@@ -8141,7 +8141,7 @@
         <v>0.27600000000000002</v>
       </c>
     </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A220" t="s">
         <v>274</v>
       </c>
@@ -8167,7 +8167,7 @@
         <v>0.27400000000000002</v>
       </c>
     </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A221" t="s">
         <v>275</v>
       </c>
@@ -8193,7 +8193,7 @@
         <v>0.27900000000000003</v>
       </c>
     </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A222" t="s">
         <v>276</v>
       </c>
@@ -8219,7 +8219,7 @@
         <v>0.35899999999999999</v>
       </c>
     </row>
-    <row r="223" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A223" t="s">
         <v>277</v>
       </c>
@@ -8245,7 +8245,7 @@
         <v>0.34499999999999997</v>
       </c>
     </row>
-    <row r="224" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A224" t="s">
         <v>278</v>
       </c>
@@ -8271,7 +8271,7 @@
         <v>0.41199999999999998</v>
       </c>
     </row>
-    <row r="225" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A225" t="s">
         <v>279</v>
       </c>
@@ -8297,7 +8297,7 @@
         <v>0.41699999999999998</v>
       </c>
     </row>
-    <row r="226" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A226" t="s">
         <v>280</v>
       </c>
@@ -8323,7 +8323,7 @@
         <v>0.27600000000000002</v>
       </c>
     </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A227" t="s">
         <v>281</v>
       </c>
@@ -8349,7 +8349,7 @@
         <v>0.38700000000000001</v>
       </c>
     </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A228" t="s">
         <v>282</v>
       </c>
@@ -8375,7 +8375,7 @@
         <v>0.58399999999999996</v>
       </c>
     </row>
-    <row r="229" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A229" t="s">
         <v>283</v>
       </c>
@@ -8401,7 +8401,7 @@
         <v>0.38900000000000001</v>
       </c>
     </row>
-    <row r="230" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A230" t="s">
         <v>284</v>
       </c>
@@ -8427,7 +8427,7 @@
         <v>0.41799999999999998</v>
       </c>
     </row>
-    <row r="231" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A231" t="s">
         <v>285</v>
       </c>
@@ -8453,7 +8453,7 @@
         <v>0.78300000000000003</v>
       </c>
     </row>
-    <row r="232" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A232" t="s">
         <v>286</v>
       </c>
@@ -8479,7 +8479,7 @@
         <v>0.60299999999999998</v>
       </c>
     </row>
-    <row r="233" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A233" t="s">
         <v>287</v>
       </c>
@@ -8505,7 +8505,7 @@
         <v>0.77800000000000002</v>
       </c>
     </row>
-    <row r="234" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A234" t="s">
         <v>288</v>
       </c>
@@ -8531,7 +8531,7 @@
         <v>0.82899999999999996</v>
       </c>
     </row>
-    <row r="235" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A235" t="s">
         <v>289</v>
       </c>
@@ -8557,7 +8557,7 @@
         <v>0.55100000000000005</v>
       </c>
     </row>
-    <row r="236" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A236" t="s">
         <v>290</v>
       </c>
@@ -8583,7 +8583,7 @@
         <v>0.41399999999999998</v>
       </c>
     </row>
-    <row r="237" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A237" t="s">
         <v>291</v>
       </c>
@@ -8609,7 +8609,7 @@
         <v>0.27100000000000002</v>
       </c>
     </row>
-    <row r="238" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A238" t="s">
         <v>292</v>
       </c>
@@ -8635,7 +8635,7 @@
         <v>0.55400000000000005</v>
       </c>
     </row>
-    <row r="239" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A239" t="s">
         <v>293</v>
       </c>
@@ -8661,7 +8661,7 @@
         <v>0.80800000000000005</v>
       </c>
     </row>
-    <row r="240" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A240" t="s">
         <v>294</v>
       </c>
@@ -8687,7 +8687,7 @@
         <v>0.81299999999999994</v>
       </c>
     </row>
-    <row r="241" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A241" t="s">
         <v>295</v>
       </c>
@@ -8713,7 +8713,7 @@
         <v>0.59499999999999997</v>
       </c>
     </row>
-    <row r="242" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A242" t="s">
         <v>296</v>
       </c>
@@ -8739,7 +8739,7 @@
         <v>0.27400000000000002</v>
       </c>
     </row>
-    <row r="243" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A243" t="s">
         <v>297</v>
       </c>
@@ -8765,7 +8765,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="244" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A244" t="s">
         <v>298</v>
       </c>
@@ -8791,7 +8791,7 @@
         <v>0.55200000000000005</v>
       </c>
     </row>
-    <row r="245" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A245" t="s">
         <v>299</v>
       </c>
@@ -8817,7 +8817,7 @@
         <v>0.78500000000000003</v>
       </c>
     </row>
-    <row r="246" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A246" t="s">
         <v>300</v>
       </c>
@@ -8843,7 +8843,7 @@
         <v>0.82099999999999995</v>
       </c>
     </row>
-    <row r="247" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A247" t="s">
         <v>301</v>
       </c>
@@ -8869,7 +8869,7 @@
         <v>0.53800000000000003</v>
       </c>
     </row>
-    <row r="248" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A248" t="s">
         <v>302</v>
       </c>
@@ -8895,7 +8895,7 @@
         <v>0.36099999999999999</v>
       </c>
     </row>
-    <row r="249" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A249" t="s">
         <v>303</v>
       </c>
@@ -8921,7 +8921,7 @@
         <v>0.54300000000000004</v>
       </c>
     </row>
-    <row r="250" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A250" t="s">
         <v>304</v>
       </c>
@@ -8947,7 +8947,7 @@
         <v>0.27200000000000002</v>
       </c>
     </row>
-    <row r="251" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A251" t="s">
         <v>305</v>
       </c>
@@ -8973,7 +8973,7 @@
         <v>0.58099999999999996</v>
       </c>
     </row>
-    <row r="252" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A252" t="s">
         <v>306</v>
       </c>
@@ -8999,7 +8999,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="253" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A253" t="s">
         <v>307</v>
       </c>
@@ -9025,7 +9025,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="254" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A254" t="s">
         <v>308</v>
       </c>
@@ -9051,7 +9051,7 @@
         <v>0.35699999999999998</v>
       </c>
     </row>
-    <row r="255" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A255" t="s">
         <v>309</v>
       </c>
@@ -9077,7 +9077,7 @@
         <v>0.60499999999999998</v>
       </c>
     </row>
-    <row r="256" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A256" t="s">
         <v>310</v>
       </c>
@@ -9103,7 +9103,7 @@
         <v>0.78300000000000003</v>
       </c>
     </row>
-    <row r="257" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A257" t="s">
         <v>311</v>
       </c>
@@ -9129,7 +9129,7 @@
         <v>0.52700000000000002</v>
       </c>
     </row>
-    <row r="258" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A258" t="s">
         <v>312</v>
       </c>
@@ -9155,7 +9155,7 @@
         <v>0.60599999999999998</v>
       </c>
     </row>
-    <row r="259" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A259" t="s">
         <v>313</v>
       </c>
@@ -9181,7 +9181,7 @@
         <v>0.41299999999999998</v>
       </c>
     </row>
-    <row r="260" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A260" t="s">
         <v>314</v>
       </c>
@@ -9207,7 +9207,7 @@
         <v>0.41799999999999998</v>
       </c>
     </row>
-    <row r="261" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A261" t="s">
         <v>315</v>
       </c>
@@ -9233,7 +9233,7 @@
         <v>0.57599999999999996</v>
       </c>
     </row>
-    <row r="262" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A262" t="s">
         <v>316</v>
       </c>
@@ -9259,7 +9259,7 @@
         <v>0.78100000000000003</v>
       </c>
     </row>
-    <row r="263" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A263" t="s">
         <v>317</v>
       </c>
@@ -9285,7 +9285,7 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="264" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A264" t="s">
         <v>318</v>
       </c>
@@ -9311,7 +9311,7 @@
         <v>0.36099999999999999</v>
       </c>
     </row>
-    <row r="265" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A265" t="s">
         <v>319</v>
       </c>
@@ -9337,7 +9337,7 @@
         <v>0.55200000000000005</v>
       </c>
     </row>
-    <row r="266" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A266" t="s">
         <v>320</v>
       </c>
@@ -9363,7 +9363,7 @@
         <v>0.35299999999999998</v>
       </c>
     </row>
-    <row r="267" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A267" t="s">
         <v>321</v>
       </c>
@@ -9389,7 +9389,7 @@
         <v>0.35499999999999998</v>
       </c>
     </row>
-    <row r="268" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A268" t="s">
         <v>322</v>
       </c>
@@ -9415,7 +9415,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="269" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A269" t="s">
         <v>323</v>
       </c>
@@ -9441,7 +9441,7 @@
         <v>0.55500000000000005</v>
       </c>
     </row>
-    <row r="270" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A270" t="s">
         <v>324</v>
       </c>
@@ -9467,7 +9467,7 @@
         <v>0.61299999999999999</v>
       </c>
     </row>
-    <row r="271" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A271" t="s">
         <v>325</v>
       </c>
@@ -9493,7 +9493,7 @@
         <v>0.27400000000000002</v>
       </c>
     </row>
-    <row r="272" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A272" t="s">
         <v>326</v>
       </c>
@@ -9519,7 +9519,7 @@
         <v>0.41399999999999998</v>
       </c>
     </row>
-    <row r="273" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A273" t="s">
         <v>327</v>
       </c>
@@ -9545,7 +9545,7 @@
         <v>0.52900000000000003</v>
       </c>
     </row>
-    <row r="274" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A274" t="s">
         <v>328</v>
       </c>
@@ -9571,7 +9571,7 @@
         <v>0.34200000000000003</v>
       </c>
     </row>
-    <row r="275" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A275" t="s">
         <v>329</v>
       </c>
@@ -9597,7 +9597,7 @@
         <v>0.52400000000000002</v>
       </c>
     </row>
-    <row r="276" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A276" t="s">
         <v>330</v>
       </c>
@@ -9623,7 +9623,7 @@
         <v>0.27600000000000002</v>
       </c>
     </row>
-    <row r="277" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A277" t="s">
         <v>331</v>
       </c>
@@ -9649,7 +9649,7 @@
         <v>0.53100000000000003</v>
       </c>
     </row>
-    <row r="278" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A278" t="s">
         <v>332</v>
       </c>
@@ -9675,7 +9675,7 @@
         <v>0.61</v>
       </c>
     </row>
-    <row r="279" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A279" t="s">
         <v>333</v>
       </c>
@@ -9701,7 +9701,7 @@
         <v>0.82299999999999995</v>
       </c>
     </row>
-    <row r="280" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A280" t="s">
         <v>334</v>
       </c>
@@ -9727,7 +9727,7 @@
         <v>0.255</v>
       </c>
     </row>
-    <row r="281" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A281" t="s">
         <v>335</v>
       </c>
@@ -9753,7 +9753,7 @@
         <v>0.40100000000000002</v>
       </c>
     </row>
-    <row r="282" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A282" t="s">
         <v>336</v>
       </c>
@@ -9779,7 +9779,7 @@
         <v>0.54700000000000004</v>
       </c>
     </row>
-    <row r="283" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A283" t="s">
         <v>337</v>
       </c>
@@ -9805,7 +9805,7 @@
         <v>0.33100000000000002</v>
       </c>
     </row>
-    <row r="284" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A284" t="s">
         <v>338</v>
       </c>
@@ -9831,7 +9831,7 @@
         <v>0.27100000000000002</v>
       </c>
     </row>
-    <row r="285" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A285" t="s">
         <v>339</v>
       </c>
@@ -9857,7 +9857,7 @@
         <v>0.59899999999999998</v>
       </c>
     </row>
-    <row r="286" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A286" t="s">
         <v>340</v>
       </c>
@@ -9883,7 +9883,7 @@
         <v>0.35099999999999998</v>
       </c>
     </row>
-    <row r="287" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A287" t="s">
         <v>341</v>
       </c>
@@ -9909,7 +9909,7 @@
         <v>0.40799999999999997</v>
       </c>
     </row>
-    <row r="288" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A288" t="s">
         <v>342</v>
       </c>
@@ -9935,7 +9935,7 @@
         <v>0.83299999999999996</v>
       </c>
     </row>
-    <row r="289" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A289" t="s">
         <v>343</v>
       </c>
@@ -9961,7 +9961,7 @@
         <v>0.35299999999999998</v>
       </c>
     </row>
-    <row r="290" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A290" t="s">
         <v>344</v>
       </c>
@@ -9987,7 +9987,7 @@
         <v>0.83299999999999996</v>
       </c>
     </row>
-    <row r="291" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A291" t="s">
         <v>345</v>
       </c>
@@ -10026,9 +10026,9 @@
       <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>45</v>
@@ -10037,7 +10037,7 @@
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>35</v>
       </c>
@@ -10054,7 +10054,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -10071,7 +10071,7 @@
         <v>2.875</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -10088,7 +10088,7 @@
         <v>2.375</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -10105,7 +10105,7 @@
         <v>1.8250000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -10135,9 +10135,9 @@
       <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10157,7 +10157,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
@@ -10177,7 +10177,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
@@ -10197,7 +10197,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
@@ -10217,7 +10217,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
@@ -10237,7 +10237,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
@@ -10257,7 +10257,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
@@ -10290,9 +10290,9 @@
       <selection sqref="A1:E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10309,7 +10309,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
@@ -10326,7 +10326,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
@@ -10343,7 +10343,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
@@ -10360,7 +10360,7 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
@@ -10377,7 +10377,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
@@ -10394,7 +10394,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
@@ -10420,11 +10420,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E3C409F-772B-49A7-B6E3-401FF4E0BC50}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -10450,7 +10450,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>30</v>
       </c>
@@ -10472,7 +10472,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="1"/>
       <c r="B3" s="1">
         <v>2</v>
@@ -10492,7 +10492,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>31</v>
       </c>
@@ -10516,7 +10516,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="1"/>
       <c r="B5" s="1">
         <v>2</v>
@@ -10538,7 +10538,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" s="1"/>
       <c r="B6" s="1">
         <v>3</v>
@@ -10558,7 +10558,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>32</v>
       </c>
@@ -10580,7 +10580,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>33</v>
       </c>
@@ -10606,7 +10606,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" s="1"/>
       <c r="B9" s="1">
         <v>2</v>
@@ -10630,7 +10630,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
@@ -10646,7 +10646,7 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>22</v>
       </c>
@@ -10662,7 +10662,7 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
@@ -10678,7 +10678,7 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
@@ -10694,7 +10694,7 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
@@ -10710,7 +10710,7 @@
       </c>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>26</v>
       </c>
@@ -10739,12 +10739,12 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="15.44140625" customWidth="1"/>
+    <col min="3" max="3" width="15.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>35</v>
       </c>
@@ -10767,7 +10767,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -10790,7 +10790,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -10813,7 +10813,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -10836,7 +10836,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -10870,9 +10870,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="1"/>
       <c r="B1" s="10" t="s">
         <v>43</v>
@@ -10880,7 +10880,7 @@
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>12</v>
@@ -10892,7 +10892,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
@@ -10900,7 +10900,7 @@
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -10914,7 +10914,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -10928,7 +10928,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
@@ -10942,7 +10942,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="57" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>51</v>
       </c>
@@ -10950,7 +10950,7 @@
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -10964,7 +10964,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -10978,7 +10978,7 @@
         <v>2070</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>

</xml_diff>